<commit_message>
add missing year values for the robs
</commit_message>
<xml_diff>
--- a/02_data/rawdata/Dataextraction_Johanna_14.08.2024.xlsx
+++ b/02_data/rawdata/Dataextraction_Johanna_14.08.2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Documents\PhD\UmbrellaMA\02_data\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0BE199B-3BD4-4A80-9B26-0EE9EF543BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04131B27-878B-48D7-B0A1-8DB4E229DE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3AAACC5A-9152-4926-B2FC-12F3D1DCD83D}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <author>tc={2D870865-A1BD-40C5-9F82-210C4FA1A8A5}</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{11D8E69E-353D-45DE-A728-9F00CC35365B}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{11D8E69E-353D-45DE-A728-9F00CC35365B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -69,7 +69,7 @@
 If studies with different populations were used in the pooled analysis, please state all (e.g. APS, NPS, SCZ)</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{E90F68CE-BF86-4A0E-B7E2-F0BF103A18BC}">
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{E90F68CE-BF86-4A0E-B7E2-F0BF103A18BC}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -77,7 +77,7 @@
     How was the target population identified? e.g. DSM-5, ICD-10, CAARMS ...</t>
       </text>
     </comment>
-    <comment ref="AG1" authorId="2" shapeId="0" xr:uid="{25C5F2AB-3489-483F-8E68-5563E0E4FD4C}">
+    <comment ref="AJ1" authorId="2" shapeId="0" xr:uid="{25C5F2AB-3489-483F-8E68-5563E0E4FD4C}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -86,7 +86,7 @@
 e.g. PANSS, DSM-5 ...</t>
       </text>
     </comment>
-    <comment ref="AH1" authorId="3" shapeId="0" xr:uid="{6C4A7145-0951-4AEA-B922-EF3A53049A45}">
+    <comment ref="AK1" authorId="3" shapeId="0" xr:uid="{6C4A7145-0951-4AEA-B922-EF3A53049A45}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -94,7 +94,7 @@
     Use Prospective or Retrospective</t>
       </text>
     </comment>
-    <comment ref="AK1" authorId="4" shapeId="0" xr:uid="{3579C19F-8CA7-49E5-A025-A44C02E786BC}">
+    <comment ref="AN1" authorId="4" shapeId="0" xr:uid="{3579C19F-8CA7-49E5-A025-A44C02E786BC}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -102,7 +102,7 @@
     use months</t>
       </text>
     </comment>
-    <comment ref="AU1" authorId="5" shapeId="0" xr:uid="{89C1D350-60DF-4EF6-9B4A-8059A1237039}">
+    <comment ref="AX1" authorId="5" shapeId="0" xr:uid="{89C1D350-60DF-4EF6-9B4A-8059A1237039}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -110,7 +110,7 @@
     These 4 purple columns are for “binary” or “raw” data that is used to calculate odds ratios. You can google “binary data for odds ratio” to get an understanding, but essentially each subject within a RF in a paper can only exist in one of these 4 purple columns, based on whether they have/do not used cannabis and whether they developed psychotic symptoms or not. This is why, in a paper that had e.g. 100 subjects, for a given risk factor, the sum total of these 4 purple columns will add up to 100.</t>
       </text>
     </comment>
-    <comment ref="CU1" authorId="6" shapeId="0" xr:uid="{2967C25E-7ECF-417F-95B7-7B187617532F}">
+    <comment ref="CX1" authorId="6" shapeId="0" xr:uid="{2967C25E-7ECF-417F-95B7-7B187617532F}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -118,7 +118,7 @@
     Make sure you are reporting the SD (and not SE, they are different!). If no SD and only SE, extract it and make a clear note.</t>
       </text>
     </comment>
-    <comment ref="CW1" authorId="7" shapeId="0" xr:uid="{5EF343A8-9211-4E48-8AA6-D42452ABDCCA}">
+    <comment ref="CZ1" authorId="7" shapeId="0" xr:uid="{5EF343A8-9211-4E48-8AA6-D42452ABDCCA}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -126,7 +126,7 @@
     Make sure you are reporting the SD (and not SE, they are different!). If no SD and only SE, extract it and make a clear note.</t>
       </text>
     </comment>
-    <comment ref="CY1" authorId="8" shapeId="0" xr:uid="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
+    <comment ref="DB1" authorId="8" shapeId="0" xr:uid="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -136,7 +136,7 @@
     hedges g</t>
       </text>
     </comment>
-    <comment ref="DB1" authorId="9" shapeId="0" xr:uid="{2D870865-A1BD-40C5-9F82-210C4FA1A8A5}">
+    <comment ref="DE1" authorId="9" shapeId="0" xr:uid="{2D870865-A1BD-40C5-9F82-210C4FA1A8A5}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="191">
   <si>
     <t xml:space="preserve">Extracted by </t>
   </si>
@@ -544,7 +544,184 @@
     <t>Lavoie</t>
   </si>
   <si>
-    <t>Henquet</t>
+    <t>CHR</t>
+  </si>
+  <si>
+    <t>20.3(3.9)</t>
+  </si>
+  <si>
+    <t>18.9(3.9)</t>
+  </si>
+  <si>
+    <t>Johanna</t>
+  </si>
+  <si>
+    <t>past year</t>
+  </si>
+  <si>
+    <t>any use</t>
+  </si>
+  <si>
+    <t>lifetime</t>
+  </si>
+  <si>
+    <t>CUD</t>
+  </si>
+  <si>
+    <t>Chi-Square = 0.78</t>
+  </si>
+  <si>
+    <t>Chi-Square = 1.05</t>
+  </si>
+  <si>
+    <t>.38</t>
+  </si>
+  <si>
+    <t>.31</t>
+  </si>
+  <si>
+    <t>prospective longitudinal cohort</t>
+  </si>
+  <si>
+    <t>no use</t>
+  </si>
+  <si>
+    <t>no CUD</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.schres.2010.09.007</t>
+  </si>
+  <si>
+    <t>SIPS, DSM,BLIPS, BSABS-P</t>
+  </si>
+  <si>
+    <t>transition to psychosis</t>
+  </si>
+  <si>
+    <t>score of 6 in one or more of the positive items of the SIPS with duration of more one week</t>
+  </si>
+  <si>
+    <t>Outcom_coded</t>
+  </si>
+  <si>
+    <t>SIPS, SCID</t>
+  </si>
+  <si>
+    <t>SIPS,SCID</t>
+  </si>
+  <si>
+    <t>Sample similar to Velthorst et al.2009</t>
+  </si>
+  <si>
+    <t>Sample similar to Velthorst et al.2010</t>
+  </si>
+  <si>
+    <t>Exclusion Criteria</t>
+  </si>
+  <si>
+    <t>hard drugs use (cocaine, heroine,amphetamines, magic,  mushrooms),iQ&lt;85,symptoms only due to drug use or organic factors, subjects who used cannabis were asked if they had a period of symptoms in which they did not use cannabis and if not they were asked to stop using for two weeks to see if symptoms continued</t>
+  </si>
+  <si>
+    <t>Cohort</t>
+  </si>
+  <si>
+    <t>Amsterdam Site of Dutch Prediction of Psychosis Study (DUPS)</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Environmental factors and social adjustment as predictors of a first psychosis in subjects at ultra high risk</t>
+  </si>
+  <si>
+    <t>Sara Dragt , Dorien H. Nieman , Doede Veltman , Hiske E. Becker Lieuwe de Haan , Don H. Linszen</t>
+  </si>
+  <si>
+    <t>The temporal dynamics of relationships between cannabis, psychosis and depression among young adults with psychotic disorders: findings from a 10-month prospective study</t>
+  </si>
+  <si>
+    <t>16-50</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Patients of the community mental health centres in the Northern Sydney Area Health Service</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>schizophrenia, schizophreniform disorder, schizoaffective disorder</t>
+  </si>
+  <si>
+    <t>psychotic symptoms</t>
+  </si>
+  <si>
+    <t>BRPS</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>10 months</t>
+  </si>
+  <si>
+    <t>36 months</t>
+  </si>
+  <si>
+    <t>0.129</t>
+  </si>
+  <si>
+    <t>0.065</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>0.033</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>prior psychotic symptoms, current depressive symptoms, sex</t>
+  </si>
+  <si>
+    <t>past month</t>
+  </si>
+  <si>
+    <t>number of days use</t>
+  </si>
+  <si>
+    <t>25.3(SE=6.4)</t>
+  </si>
+  <si>
+    <t>monthly measures</t>
+  </si>
+  <si>
+    <t>univariate GEE, multiple regression</t>
+  </si>
+  <si>
+    <t>within-subjects design, several measures of cannabis use and psychosis over 10 months, adjusted and unadjusted unstandardized betas</t>
+  </si>
+  <si>
+    <t>doi:10.1017/S0033291707009956</t>
+  </si>
+  <si>
+    <t>Pittsburgh Youth Study</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>past month and past year</t>
   </si>
 </sst>
 </file>
@@ -592,12 +769,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,6 +908,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -871,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1038,6 +1228,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1379,7 +1573,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="I1" dT="2021-07-21T20:28:28.02" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{11D8E69E-353D-45DE-A728-9F00CC35365B}">
+  <threadedComment ref="K1" dT="2021-07-21T20:28:28.02" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{11D8E69E-353D-45DE-A728-9F00CC35365B}">
     <text>In which population is cannabis consumption and the outcome measured?
 Please use the following Abbrevations:
 HP = Healthy individuals (general population)
@@ -1393,35 +1587,35 @@
 APS = Affective Psychosis ( i.e. MDD with psychotic features, bipolar disorder with psychotic features...)
 If studies with different populations were used in the pooled analysis, please state all (e.g. APS, NPS, SCZ)</text>
   </threadedComment>
-  <threadedComment ref="K1" dT="2021-07-21T20:29:37.10" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{E90F68CE-BF86-4A0E-B7E2-F0BF103A18BC}">
+  <threadedComment ref="M1" dT="2021-07-21T20:29:37.10" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{E90F68CE-BF86-4A0E-B7E2-F0BF103A18BC}">
     <text>How was the target population identified? e.g. DSM-5, ICD-10, CAARMS ...</text>
   </threadedComment>
-  <threadedComment ref="AG1" dT="2021-07-21T21:16:32.43" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{25C5F2AB-3489-483F-8E68-5563E0E4FD4C}">
+  <threadedComment ref="AJ1" dT="2021-07-21T21:16:32.43" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{25C5F2AB-3489-483F-8E68-5563E0E4FD4C}">
     <text>How was the outcome (transitioning to psychosis, psychotic symptoms, subclinical psychotic symptoms etc measured? 
 e.g. PANSS, DSM-5 ...</text>
   </threadedComment>
-  <threadedComment ref="AH1" dT="2020-01-30T15:47:15.22" personId="{CD06699D-F9B0-4E16-B3C7-56F9D6109F9B}" id="{6C4A7145-0951-4AEA-B922-EF3A53049A45}">
+  <threadedComment ref="AK1" dT="2020-01-30T15:47:15.22" personId="{CD06699D-F9B0-4E16-B3C7-56F9D6109F9B}" id="{6C4A7145-0951-4AEA-B922-EF3A53049A45}">
     <text>Use Prospective or Retrospective</text>
   </threadedComment>
-  <threadedComment ref="AK1" dT="2021-07-27T11:55:01.30" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{3579C19F-8CA7-49E5-A025-A44C02E786BC}">
+  <threadedComment ref="AN1" dT="2021-07-27T11:55:01.30" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{3579C19F-8CA7-49E5-A025-A44C02E786BC}">
     <text>use months</text>
   </threadedComment>
-  <threadedComment ref="AU1" dT="2021-07-22T10:51:44.19" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{89C1D350-60DF-4EF6-9B4A-8059A1237039}">
+  <threadedComment ref="AX1" dT="2021-07-22T10:51:44.19" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{89C1D350-60DF-4EF6-9B4A-8059A1237039}">
     <text>These 4 purple columns are for “binary” or “raw” data that is used to calculate odds ratios. You can google “binary data for odds ratio” to get an understanding, but essentially each subject within a RF in a paper can only exist in one of these 4 purple columns, based on whether they have/do not used cannabis and whether they developed psychotic symptoms or not. This is why, in a paper that had e.g. 100 subjects, for a given risk factor, the sum total of these 4 purple columns will add up to 100.</text>
   </threadedComment>
-  <threadedComment ref="CU1" dT="2021-07-22T11:02:39.21" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{2967C25E-7ECF-417F-95B7-7B187617532F}">
+  <threadedComment ref="CX1" dT="2021-07-22T11:02:39.21" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{2967C25E-7ECF-417F-95B7-7B187617532F}">
     <text>Make sure you are reporting the SD (and not SE, they are different!). If no SD and only SE, extract it and make a clear note.</text>
   </threadedComment>
-  <threadedComment ref="CW1" dT="2021-07-22T11:02:44.92" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{5EF343A8-9211-4E48-8AA6-D42452ABDCCA}">
+  <threadedComment ref="CZ1" dT="2021-07-22T11:02:44.92" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{5EF343A8-9211-4E48-8AA6-D42452ABDCCA}">
     <text>Make sure you are reporting the SD (and not SE, they are different!). If no SD and only SE, extract it and make a clear note.</text>
   </threadedComment>
-  <threadedComment ref="CY1" dT="2021-08-02T22:35:31.98" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
+  <threadedComment ref="DB1" dT="2021-08-02T22:35:31.98" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
     <text>What kind of stanardized mean difference is that? e.g. Cohen's d , Glass' delta</text>
   </threadedComment>
-  <threadedComment ref="CY1" dT="2021-08-03T00:07:06.64" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{7B2A2722-2B10-4D98-A067-59E16A31DB60}" parentId="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
+  <threadedComment ref="DB1" dT="2021-08-03T00:07:06.64" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{7B2A2722-2B10-4D98-A067-59E16A31DB60}" parentId="{3AD5F74E-72C6-4EE6-BBBB-A14FAD1763B1}">
     <text>hedges g</text>
   </threadedComment>
-  <threadedComment ref="DB1" dT="2021-08-02T23:37:28.46" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{2D870865-A1BD-40C5-9F82-210C4FA1A8A5}">
+  <threadedComment ref="DE1" dT="2021-08-02T23:37:28.46" personId="{6B838454-0208-4B7B-8DDE-158AA8B1084E}" id="{2D870865-A1BD-40C5-9F82-210C4FA1A8A5}">
     <text>what is the p-value for the SMD?</text>
   </threadedComment>
 </ThreadedComments>
@@ -1429,24 +1623,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BCF2B3-B3E3-4473-A74F-1557EB7AB89B}">
-  <dimension ref="A1:DS11"/>
+  <dimension ref="A1:DW11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D13"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="110.26953125" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" customWidth="1"/>
-    <col min="18" max="18" width="21.26953125" customWidth="1"/>
-    <col min="19" max="19" width="24.6328125" customWidth="1"/>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="5" max="5" width="84.453125" customWidth="1"/>
+    <col min="6" max="6" width="129.90625" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" customWidth="1"/>
+    <col min="10" max="10" width="28.81640625" customWidth="1"/>
+    <col min="13" max="13" width="23.36328125" customWidth="1"/>
+    <col min="16" max="16" width="24.453125" customWidth="1"/>
+    <col min="17" max="17" width="35" customWidth="1"/>
+    <col min="18" max="18" width="46.08984375" customWidth="1"/>
+    <col min="20" max="20" width="21.26953125" customWidth="1"/>
+    <col min="21" max="21" width="24.6328125" customWidth="1"/>
+    <col min="22" max="23" width="16.1796875" customWidth="1"/>
+    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="29" max="29" width="18.08984375" customWidth="1"/>
+    <col min="31" max="31" width="21.1796875" customWidth="1"/>
+    <col min="32" max="32" width="19.08984375" customWidth="1"/>
+    <col min="34" max="34" width="72.90625" customWidth="1"/>
+    <col min="35" max="35" width="19.453125" customWidth="1"/>
+    <col min="36" max="36" width="9.36328125" customWidth="1"/>
+    <col min="39" max="39" width="36.1796875" customWidth="1"/>
+    <col min="48" max="48" width="9.36328125" customWidth="1"/>
+    <col min="54" max="54" width="13" customWidth="1"/>
+    <col min="117" max="117" width="8.1796875" customWidth="1"/>
+    <col min="118" max="118" width="51" customWidth="1"/>
+    <col min="119" max="119" width="31.36328125" customWidth="1"/>
+    <col min="120" max="120" width="31.08984375" customWidth="1"/>
+    <col min="122" max="122" width="21.90625" customWidth="1"/>
+    <col min="127" max="127" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:123" s="55" customFormat="1" ht="49.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:127" s="55" customFormat="1" ht="49.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
         <v>69</v>
       </c>
@@ -1462,443 +1680,757 @@
       <c r="E1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="T1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="U1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="V1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AC1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AF1" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AG1" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AK1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="29" t="s">
+      <c r="AL1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AM1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="30" t="s">
+      <c r="AO1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="AM1" s="31" t="s">
+      <c r="AP1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AN1" s="32" t="s">
+      <c r="AQ1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="AO1" s="33" t="s">
+      <c r="AR1" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" s="33" t="s">
+      <c r="AS1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" s="33" t="s">
+      <c r="AT1" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" s="34" t="s">
+      <c r="AU1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="34" t="s">
+      <c r="AV1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="AT1" s="35" t="s">
+      <c r="AW1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AX1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AV1" s="13" t="s">
+      <c r="AY1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="AZ1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="BA1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AY1" s="13" t="s">
+      <c r="BB1" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BC1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="BA1" s="36" t="s">
+      <c r="BD1" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="BB1" s="37" t="s">
+      <c r="BE1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="BC1" s="37" t="s">
+      <c r="BF1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="BD1" s="37" t="s">
+      <c r="BG1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="BE1" s="38" t="s">
+      <c r="BH1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="BF1" s="39" t="s">
+      <c r="BI1" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="BG1" s="40" t="s">
+      <c r="BJ1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="BH1" s="40" t="s">
+      <c r="BK1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="BI1" s="40" t="s">
+      <c r="BL1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="BJ1" s="40" t="s">
+      <c r="BM1" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="BK1" s="15" t="s">
+      <c r="BN1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="BL1" s="16" t="s">
+      <c r="BO1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="BM1" s="16" t="s">
+      <c r="BP1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="BN1" s="16" t="s">
+      <c r="BQ1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="BO1" s="16" t="s">
+      <c r="BR1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="BP1" s="41" t="s">
+      <c r="BS1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="BQ1" s="36" t="s">
+      <c r="BT1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="BR1" s="37" t="s">
+      <c r="BU1" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="BS1" s="37" t="s">
+      <c r="BV1" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="BT1" s="37" t="s">
+      <c r="BW1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="BU1" s="38" t="s">
+      <c r="BX1" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="BV1" s="17" t="s">
+      <c r="BY1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="BW1" s="39" t="s">
+      <c r="BZ1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="BX1" s="40" t="s">
+      <c r="CA1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="BY1" s="40" t="s">
+      <c r="CB1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="BZ1" s="40" t="s">
+      <c r="CC1" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="CA1" s="40" t="s">
+      <c r="CD1" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="CB1" s="18" t="s">
+      <c r="CE1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="CC1" s="42" t="s">
+      <c r="CF1" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="CD1" s="41" t="s">
+      <c r="CG1" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="CE1" s="41" t="s">
+      <c r="CH1" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="CF1" s="41" t="s">
+      <c r="CI1" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="CG1" s="41" t="s">
+      <c r="CJ1" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="CH1" s="41" t="s">
+      <c r="CK1" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="CI1" s="43" t="s">
+      <c r="CL1" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="CJ1" s="44" t="s">
+      <c r="CM1" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="CK1" s="45" t="s">
+      <c r="CN1" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="CL1" s="45" t="s">
+      <c r="CO1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="CM1" s="46" t="s">
+      <c r="CP1" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="CN1" s="47" t="s">
+      <c r="CQ1" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="CO1" s="47" t="s">
+      <c r="CR1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="CP1" s="47" t="s">
+      <c r="CS1" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="CQ1" s="47" t="s">
+      <c r="CT1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="CR1" s="47" t="s">
+      <c r="CU1" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="CS1" s="47" t="s">
+      <c r="CV1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="CT1" s="19" t="s">
+      <c r="CW1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="CU1" s="20" t="s">
+      <c r="CX1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="CV1" s="20" t="s">
+      <c r="CY1" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="CW1" s="48" t="s">
+      <c r="CZ1" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="CX1" s="49" t="s">
+      <c r="DA1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="CY1" s="49" t="s">
+      <c r="DB1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="CZ1" s="21" t="s">
+      <c r="DC1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="DA1" s="21" t="s">
+      <c r="DD1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="DB1" s="21" t="s">
+      <c r="DE1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="DC1" s="50" t="s">
+      <c r="DF1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="DD1" s="50" t="s">
+      <c r="DG1" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="DE1" s="50" t="s">
+      <c r="DH1" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="DF1" s="50" t="s">
+      <c r="DI1" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="DG1" s="50" t="s">
+      <c r="DJ1" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="DH1" s="50" t="s">
+      <c r="DK1" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="DI1" s="50" t="s">
+      <c r="DL1" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="DJ1" s="50" t="s">
+      <c r="DM1" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="DK1" s="50" t="s">
+      <c r="DN1" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="DL1" s="50" t="s">
+      <c r="DO1" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="DM1" s="51" t="s">
+      <c r="DP1" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="DN1" s="51" t="s">
+      <c r="DQ1" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="DO1" s="51" t="s">
+      <c r="DR1" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="DP1" s="51" t="s">
+      <c r="DS1" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="DQ1" s="52" t="s">
+      <c r="DT1" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="DR1" s="53" t="s">
+      <c r="DU1" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="DS1" s="54" t="s">
+      <c r="DV1" s="54" t="s">
         <v>122</v>
       </c>
+      <c r="DW1" s="55" t="s">
+        <v>156</v>
+      </c>
     </row>
-    <row r="2" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F2" t="s">
+    <row r="2" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" t="s">
         <v>123</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F3" t="s">
+    <row r="3" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" t="s">
         <v>123</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F4" t="s">
+    <row r="4" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" t="s">
         <v>124</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F5" t="s">
+    <row r="5" spans="1:127" s="56" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="56">
         <v>2015</v>
       </c>
+      <c r="J5" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="W5" s="56">
+        <v>100</v>
+      </c>
+      <c r="Z5" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC5" s="56" t="s">
+        <v>182</v>
+      </c>
     </row>
-    <row r="6" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F6" t="s">
+    <row r="6" spans="1:127" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="58">
         <v>2007</v>
       </c>
+      <c r="I6" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="L6" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="N6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y6" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z6" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA6" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC6" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH6" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ6" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK6" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM6" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN6" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="AO6" s="58">
+        <v>70</v>
+      </c>
+      <c r="DF6" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="DG6" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="DH6" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="DI6" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="DJ6" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="DM6" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="DN6" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="DO6" s="58" t="s">
+        <v>185</v>
+      </c>
     </row>
-    <row r="7" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F7" t="s">
+    <row r="7" spans="1:127" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="G7" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="57">
         <v>2011</v>
       </c>
+      <c r="I7" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="J7" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="K7" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="P7" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q7" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="X7" s="57">
+        <v>72</v>
+      </c>
+      <c r="Z7" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA7" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB7" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH7" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI7" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ7" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK7" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM7" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN7" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="AO7" s="57">
+        <v>72</v>
+      </c>
+      <c r="AP7" s="57">
+        <v>21</v>
+      </c>
+      <c r="AU7" s="57">
+        <v>19</v>
+      </c>
+      <c r="AV7" s="57">
+        <v>53</v>
+      </c>
+      <c r="AX7" s="57">
+        <v>4</v>
+      </c>
+      <c r="AZ7" s="57">
+        <v>17</v>
+      </c>
+      <c r="DR7" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="DS7" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="DW7" s="57" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="8" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F8" t="s">
+    <row r="8" spans="1:127" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="57">
+        <v>2011</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8" s="57" t="s">
+        <v>159</v>
+      </c>
+      <c r="K8" s="57" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="P8" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="X8" s="57">
+        <v>72</v>
+      </c>
+      <c r="Z8" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA8" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB8" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH8" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI8" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ8" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK8" s="57" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM8" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN8" s="57" t="s">
+        <v>173</v>
+      </c>
+      <c r="AO8" s="57">
+        <v>72</v>
+      </c>
+      <c r="AP8" s="57">
+        <v>22</v>
+      </c>
+      <c r="AU8" s="57">
+        <v>19</v>
+      </c>
+      <c r="AV8" s="57">
+        <v>53</v>
+      </c>
+      <c r="AX8" s="57">
+        <v>4</v>
+      </c>
+      <c r="AZ8" s="57">
+        <v>18</v>
+      </c>
+      <c r="DR8" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="DS8" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="DW8" s="57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" t="s">
         <v>128</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F9" t="s">
+    <row r="10" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" t="s">
         <v>129</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F10" t="s">
+    <row r="11" spans="1:127" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" t="s">
         <v>130</v>
       </c>
-      <c r="G10">
+      <c r="H11">
         <v>2014</v>
-      </c>
-    </row>
-    <row r="11" spans="1:123" x14ac:dyDescent="0.35">
-      <c r="F11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G11">
-        <v>2004</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>